<commit_message>
Tested different parameters for Weibull in version 6Weib
</commit_message>
<xml_diff>
--- a/data/Parameters.xlsx
+++ b/data/Parameters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="160" windowWidth="25360" windowHeight="15300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="160" windowWidth="25360" windowHeight="15300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HR and Stage" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
   <si>
     <t>ER+ S1</t>
   </si>
@@ -408,6 +408,33 @@
   </si>
   <si>
     <t>(c)</t>
+  </si>
+  <si>
+    <t>Weibull calculation</t>
+  </si>
+  <si>
+    <t>S(5)</t>
+  </si>
+  <si>
+    <t>S(10)</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>http://www.johndcook.com/quantiles_parameters.pdf</t>
   </si>
 </sst>
 </file>
@@ -546,9 +573,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -674,7 +703,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="82">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -714,6 +743,7 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -753,6 +783,7 @@
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1745,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2435,6 +2466,95 @@
         <v>0.12117369138229669</v>
       </c>
     </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35">
+        <f>D16</f>
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="C35">
+        <f>D17</f>
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="D35">
+        <f>1-B35</f>
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="E35">
+        <f>1-C35</f>
+        <v>0.55299999999999994</v>
+      </c>
+      <c r="F35">
+        <f>(LN(-LN(1-E35))-LN(-LN(1-D35)))/(LN(10)-LN(5))</f>
+        <v>0.65180701550007369</v>
+      </c>
+      <c r="G35">
+        <f>5/(-LN(1-D35))^(1/F35)</f>
+        <v>13.943276836384568</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <f>D4</f>
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="C36">
+        <f>D5</f>
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="D36">
+        <f>1-B36</f>
+        <v>9.3999999999999972E-2</v>
+      </c>
+      <c r="E36">
+        <f>1-C36</f>
+        <v>0.18200000000000005</v>
+      </c>
+      <c r="F36">
+        <f>(LN(-LN(1-E36))-LN(-LN(1-D36)))/(LN(10)-LN(5))</f>
+        <v>1.0250714343850138</v>
+      </c>
+      <c r="G36">
+        <f>5/(-LN(1-D36))^(1/F36)</f>
+        <v>47.861584157189903</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2450,7 +2570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>